<commit_message>
updated data and graph.
</commit_message>
<xml_diff>
--- a/resources/Final Results/FirstGuess-Results.xlsx
+++ b/resources/Final Results/FirstGuess-Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deard\Documents\Diss\Minesweeper-Assistant\resources\Final Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBA866F-4FDB-49B4-B763-23333F843B3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F96D148-EDF2-4092-B458-9B68CF200225}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12588" yWindow="2316" windowWidth="8676" windowHeight="8964" xr2:uid="{5BEA2355-FD2A-4A91-A407-782DEC419AB2}"/>
   </bookViews>
@@ -902,7 +902,7 @@
                   <c:v>0.66678800000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53962900000000003</c:v>
+                  <c:v>0.50314499999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.32570399999999999</c:v>
@@ -990,7 +990,7 @@
                   <c:v>0.59832300000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44447799999999998</c:v>
+                  <c:v>0.42375699999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.249915</c:v>
@@ -1078,7 +1078,7 @@
                   <c:v>0.49864599999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32892100000000002</c:v>
+                  <c:v>0.31222</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.15432199999999999</c:v>
@@ -2768,8 +2768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36ACA77B-069B-4599-A790-C2BFB1452F1E}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2870,7 +2870,7 @@
         <v>0.66678800000000005</v>
       </c>
       <c r="C11" s="1">
-        <v>0.53962900000000003</v>
+        <v>0.50314499999999995</v>
       </c>
       <c r="D11" s="1">
         <v>0.32570399999999999</v>
@@ -2884,7 +2884,7 @@
         <v>0.59832300000000005</v>
       </c>
       <c r="C12" s="1">
-        <v>0.44447799999999998</v>
+        <v>0.42375699999999999</v>
       </c>
       <c r="D12" s="1">
         <v>0.249915</v>
@@ -2898,7 +2898,7 @@
         <v>0.49864599999999998</v>
       </c>
       <c r="C13" s="1">
-        <v>0.32892100000000002</v>
+        <v>0.31222</v>
       </c>
       <c r="D13" s="1">
         <v>0.15432199999999999</v>

</xml_diff>